<commit_message>
Update ILED paper scenario results
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIM-2.0\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5E5AC8-6A99-402E-AD88-DE0AFADC84E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4CC272-783F-4708-92ED-B82517C62AED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="819" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1450" yWindow="830" windowWidth="14400" windowHeight="7360" tabRatio="819" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="64" r:id="rId1"/>
@@ -2263,16 +2263,16 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="60.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" customWidth="1"/>
+    <col min="5" max="5" width="60.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>232</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36">
         <v>44237</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36">
         <v>44232</v>
       </c>
@@ -2334,9 +2334,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -2429,9 +2429,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>0.12635353241295499</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>0.24100352965976199</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -2606,9 +2606,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -2703,12 +2703,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>0.20963817697789</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>0.29754218668175703</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -2883,9 +2883,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -2978,9 +2978,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>1.2457230310998201E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>1.06776419273959E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -3157,9 +3157,9 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -3254,9 +3254,9 @@
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -3352,40 +3352,40 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" style="8" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="3.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.54296875" style="8" customWidth="1"/>
+    <col min="25" max="25" width="6.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.1796875" style="8" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="8"/>
+    <col min="29" max="29" width="5.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.1796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
       <c r="C3" s="9" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -3499,12 +3499,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
         <v>13</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>17</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>21</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>25</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>27</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>29</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>31</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>33</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>35</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>37</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>39</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>41</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>43</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>45</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>47</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>49</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>51</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>53</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>55</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>57</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>59</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>61</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>63</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>65</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>67</v>
       </c>
@@ -4119,43 +4119,43 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.26953125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="3.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="2.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" customWidth="1"/>
+    <col min="8" max="8" width="2.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="3.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="3.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="3.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="2.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="2.7265625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:27" ht="13" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -4179,7 +4179,7 @@
       <c r="Z3"/>
       <c r="AA3"/>
     </row>
-    <row r="4" spans="2:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
@@ -4225,7 +4225,7 @@
       <c r="Z4"/>
       <c r="AA4"/>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:27" ht="13" x14ac:dyDescent="0.3">
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
@@ -4257,7 +4257,7 @@
       <c r="Z5"/>
       <c r="AA5"/>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -4277,7 +4277,7 @@
       <c r="Z6"/>
       <c r="AA6"/>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -4315,18 +4315,18 @@
       <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="16"/>
-    <col min="6" max="6" width="12.85546875" style="16" customWidth="1"/>
-    <col min="7" max="15" width="9.140625" style="16"/>
-    <col min="16" max="16" width="11.42578125" style="16" customWidth="1"/>
-    <col min="17" max="25" width="9.140625" style="16"/>
-    <col min="26" max="26" width="11.7109375" style="16" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="5" width="9.1796875" style="16"/>
+    <col min="6" max="6" width="12.81640625" style="16" customWidth="1"/>
+    <col min="7" max="15" width="9.1796875" style="16"/>
+    <col min="16" max="16" width="11.453125" style="16" customWidth="1"/>
+    <col min="17" max="25" width="9.1796875" style="16"/>
+    <col min="26" max="26" width="11.7265625" style="16" customWidth="1"/>
+    <col min="27" max="16384" width="9.1796875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:30" ht="23.5" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
         <v>91</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="2:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:30" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
         <v>85</v>
       </c>
@@ -4372,7 +4372,7 @@
       <c r="AC3" s="18"/>
       <c r="AD3" s="18"/>
     </row>
-    <row r="4" spans="2:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
         <v>68</v>
       </c>
@@ -4455,7 +4455,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:30" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="26" t="s">
         <v>77</v>
       </c>
@@ -4514,7 +4514,7 @@
       <c r="AC5" s="28"/>
       <c r="AD5" s="28"/>
     </row>
-    <row r="6" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:30" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="20"/>
@@ -4544,7 +4544,7 @@
       <c r="AC6" s="28"/>
       <c r="AD6" s="28"/>
     </row>
-    <row r="8" spans="2:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:30" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
         <v>87</v>
       </c>
@@ -4568,7 +4568,7 @@
       <c r="S8" s="18"/>
       <c r="T8" s="18"/>
     </row>
-    <row r="9" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
         <v>68</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:30" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B10" s="26" t="s">
         <v>77</v>
       </c>
@@ -4664,7 +4664,7 @@
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
     </row>
-    <row r="13" spans="2:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:30" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>108</v>
       </c>
@@ -4688,7 +4688,7 @@
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
     </row>
-    <row r="14" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>68</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:30" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B15" s="26" t="s">
         <v>77</v>
       </c>
@@ -4784,7 +4784,7 @@
       <c r="S15" s="28"/>
       <c r="T15" s="28"/>
     </row>
-    <row r="18" spans="2:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:20" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
         <v>118</v>
       </c>
@@ -4808,7 +4808,7 @@
       <c r="S18" s="18"/>
       <c r="T18" s="18"/>
     </row>
-    <row r="19" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="19" t="s">
         <v>68</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B20" s="26" t="s">
         <v>77</v>
       </c>
@@ -4904,7 +4904,7 @@
       <c r="S20" s="28"/>
       <c r="T20" s="28"/>
     </row>
-    <row r="23" spans="2:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:20" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>119</v>
       </c>
@@ -4928,7 +4928,7 @@
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="19" t="s">
         <v>68</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B25" s="26" t="s">
         <v>77</v>
       </c>
@@ -5024,7 +5024,7 @@
       <c r="S25" s="28"/>
       <c r="T25" s="28"/>
     </row>
-    <row r="28" spans="2:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:20" ht="14.5" x14ac:dyDescent="0.25">
       <c r="L28" s="17" t="s">
         <v>173</v>
       </c>
@@ -5037,7 +5037,7 @@
       <c r="S28" s="18"/>
       <c r="T28" s="18"/>
     </row>
-    <row r="29" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L29" s="19" t="s">
         <v>68</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="L30" s="26" t="s">
         <v>77</v>
       </c>
@@ -5087,7 +5087,7 @@
       <c r="S30" s="28"/>
       <c r="T30" s="28"/>
     </row>
-    <row r="33" spans="12:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="12:20" ht="14.5" x14ac:dyDescent="0.25">
       <c r="L33" s="17" t="s">
         <v>174</v>
       </c>
@@ -5100,7 +5100,7 @@
       <c r="S33" s="18"/>
       <c r="T33" s="18"/>
     </row>
-    <row r="34" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="12:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L34" s="19" t="s">
         <v>68</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="12:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="12:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="L35" s="26" t="s">
         <v>77</v>
       </c>
@@ -5168,33 +5168,33 @@
       <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="22" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="22" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="22"/>
-    <col min="10" max="10" width="13.140625" style="22" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="37.81640625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="22.7265625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.26953125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="22"/>
+    <col min="10" max="10" width="13.1796875" style="22" customWidth="1"/>
+    <col min="11" max="11" width="15.1796875" style="22" customWidth="1"/>
     <col min="12" max="12" width="13" style="22" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="22"/>
+    <col min="13" max="16384" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="23.5" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="H2" s="23"/>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>243</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>70</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>248</v>
       </c>
@@ -5250,7 +5250,7 @@
       <c r="K5" s="30"/>
       <c r="L5" s="31"/>
     </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
         <v>1</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>0.117199391171994</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>1</v>
       </c>
@@ -5320,7 +5320,7 @@
         <v>1.1270833191729201E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
         <v>1</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>6.7195931921959296E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
         <v>244</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>1.18630136986301E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="32" t="s">
         <v>244</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>1.0896637608966401E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="33" t="s">
         <v>244</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>0.956481782990526</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="32" t="s">
         <v>244</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
         <v>1</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>R-S*_Apt_PEA*</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="32" t="s">
         <v>1</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>R-S*_Apt_SMF*</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="33" t="s">
         <v>244</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="32" t="s">
         <v>1</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>112</v>
       </c>
@@ -5620,7 +5620,7 @@
       <c r="K17" s="30"/>
       <c r="L17" s="31"/>
     </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="32" t="s">
         <v>1</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>0.20963817697789</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="33" t="s">
         <v>1</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>0.29754218668175703</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="32" t="s">
         <v>1</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>0.49011428261671702</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="33" t="s">
         <v>244</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>0.12635353241295499</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="32" t="s">
         <v>244</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>0.24100352965976199</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="33" t="s">
         <v>244</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>0.29839165082681302</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="33" t="s">
         <v>244</v>
       </c>
@@ -5843,7 +5843,7 @@
       <c r="K24" s="33"/>
       <c r="L24" s="33"/>
     </row>
-    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="32" t="s">
         <v>244</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>R-S*_Att_GAS*</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
         <v>1</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>R-S*_Att_PEA*</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="32" t="s">
         <v>1</v>
       </c>
@@ -5915,7 +5915,7 @@
         <v>R-S*_Att_SMF*</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="33" t="s">
         <v>244</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>R-S*_Att_WOO*</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="33" t="s">
         <v>244</v>
       </c>
@@ -5955,7 +5955,7 @@
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
     </row>
-    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="32" t="s">
         <v>1</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>R-S*_Att_HET*</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
         <v>113</v>
       </c>
@@ -5991,7 +5991,7 @@
       <c r="G31" s="30"/>
       <c r="H31" s="30"/>
     </row>
-    <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="32" t="s">
         <v>1</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>R-S*_Det_COA*</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="33" t="s">
         <v>1</v>
       </c>
@@ -6040,7 +6040,7 @@
       </c>
       <c r="I33" s="25"/>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="32" t="s">
         <v>1</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>R-S*_Det_ETH*</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="33" t="s">
         <v>244</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>R-S*_Det_LPG*</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="32" t="s">
         <v>244</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>R-S*_Det_ELC*</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="33" t="s">
         <v>244</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>R-S*_Det_KER*</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="33" t="s">
         <v>244</v>
       </c>
@@ -6152,7 +6152,7 @@
       <c r="G38" s="33"/>
       <c r="H38" s="33"/>
     </row>
-    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="32" t="s">
         <v>244</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>R-S*_Det_GAS*</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="33" t="s">
         <v>1</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>R-S*_Det_PEA*</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="32" t="s">
         <v>1</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>R-S*_Det_SMF*</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="33" t="s">
         <v>244</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>R-S*_Det_WOO*</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="33" t="s">
         <v>244</v>
       </c>
@@ -6264,7 +6264,7 @@
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
     </row>
-    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="32" t="s">
         <v>1</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>R-S*_Det_HET*</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
         <v>251</v>
       </c>
@@ -6299,7 +6299,7 @@
       <c r="G45" s="30"/>
       <c r="H45" s="30"/>
     </row>
-    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="32" t="s">
         <v>1</v>
       </c>
@@ -6326,7 +6326,7 @@
         <v>R-S*_Apt_COA*</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="33" t="s">
         <v>1</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>R-S*_Apt_BDL*</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="32" t="s">
         <v>1</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>R-S*_Apt_ETH*</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="33" t="s">
         <v>198</v>
       </c>
@@ -6407,7 +6407,7 @@
         <v>R-S*_Apt_LPG*</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="32" t="s">
         <v>198</v>
       </c>
@@ -6434,7 +6434,7 @@
         <v>R-S*_Apt_ELC*</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="33" t="s">
         <v>198</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>R-S*_Apt_KER*</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="32" t="s">
         <v>198</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>R-S*_Apt_GAS*</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="33" t="s">
         <v>1</v>
       </c>
@@ -6515,7 +6515,7 @@
         <v>R-S*_Apt_PEA*</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" s="32" t="s">
         <v>1</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>R-S*_Apt_SMF*</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A55" s="33" t="s">
         <v>198</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>R-S*_Apt_WOO*</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="32" t="s">
         <v>198</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>R-S*_Apt_HET*</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A57" s="29" t="s">
         <v>250</v>
       </c>
@@ -6608,7 +6608,7 @@
       <c r="G57" s="30"/>
       <c r="H57" s="30"/>
     </row>
-    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="32" t="s">
         <v>1</v>
       </c>
@@ -6635,7 +6635,7 @@
         <v>R-S*_Att_COA*</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" s="33" t="s">
         <v>1</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>R-S*_Att_BDL*</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A60" s="32" t="s">
         <v>1</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>R-S*_Att_ETH*</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A61" s="33" t="s">
         <v>198</v>
       </c>
@@ -6716,7 +6716,7 @@
         <v>R-S*_Att_LPG*</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A62" s="32" t="s">
         <v>198</v>
       </c>
@@ -6743,7 +6743,7 @@
         <v>R-S*_Att_ELC*</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A63" s="33" t="s">
         <v>198</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>R-S*_Att_KER*</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A64" s="33" t="s">
         <v>198</v>
       </c>
@@ -6789,7 +6789,7 @@
       <c r="G64" s="33"/>
       <c r="H64" s="33"/>
     </row>
-    <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A65" s="32" t="s">
         <v>198</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>R-S*_Att_GAS*</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A66" s="33" t="s">
         <v>1</v>
       </c>
@@ -6843,7 +6843,7 @@
         <v>R-S*_Att_PEA*</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A67" s="32" t="s">
         <v>1</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>R-S*_Att_SMF*</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A68" s="33" t="s">
         <v>198</v>
       </c>
@@ -6897,7 +6897,7 @@
         <v>R-S*_Att_WOO*</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A69" s="33" t="s">
         <v>198</v>
       </c>
@@ -6916,7 +6916,7 @@
       <c r="G69" s="33"/>
       <c r="H69" s="33"/>
     </row>
-    <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A70" s="32" t="s">
         <v>198</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>R-S*_Att_HET*</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
         <v>249</v>
       </c>
@@ -6955,7 +6955,7 @@
       <c r="G71" s="30"/>
       <c r="H71" s="30"/>
     </row>
-    <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A72" s="32" t="s">
         <v>1</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>R-S*_Det_COA*</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A73" s="33" t="s">
         <v>1</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>R-S*_Det_BDL*</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A74" s="32" t="s">
         <v>1</v>
       </c>
@@ -7036,7 +7036,7 @@
         <v>R-S*_Det_ETH*</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A75" s="33" t="s">
         <v>198</v>
       </c>
@@ -7063,7 +7063,7 @@
         <v>R-S*_Det_LPG*</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A76" s="32" t="s">
         <v>198</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>R-S*_Det_ELC*</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A77" s="33" t="s">
         <v>198</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>R-S*_Det_KER*</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A78" s="33" t="s">
         <v>198</v>
       </c>
@@ -7136,7 +7136,7 @@
       <c r="G78" s="33"/>
       <c r="H78" s="33"/>
     </row>
-    <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A79" s="32" t="s">
         <v>198</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>R-S*_Det_GAS*</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A80" s="33" t="s">
         <v>1</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>R-S*_Det_PEA*</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A81" s="32" t="s">
         <v>1</v>
       </c>
@@ -7217,7 +7217,7 @@
         <v>R-S*_Det_SMF*</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A82" s="33" t="s">
         <v>198</v>
       </c>
@@ -7244,7 +7244,7 @@
         <v>R-S*_Det_WOO*</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A83" s="33" t="s">
         <v>198</v>
       </c>
@@ -7263,7 +7263,7 @@
       <c r="G83" s="33"/>
       <c r="H83" s="33"/>
     </row>
-    <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A84" s="32" t="s">
         <v>198</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>R-S*_Det_HET*</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A85" s="29" t="s">
         <v>115</v>
       </c>
@@ -7301,7 +7301,7 @@
       <c r="G85" s="30"/>
       <c r="H85" s="30"/>
     </row>
-    <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A86" s="32" t="s">
         <v>1</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>R-WH_Apt_COA*</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A87" s="33" t="s">
         <v>1</v>
       </c>
@@ -7349,7 +7349,7 @@
         <v>R-WH_Apt_BDL*</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A88" s="32" t="s">
         <v>1</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>R-WH_Apt_ETH*</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A89" s="33" t="s">
         <v>1</v>
       </c>
@@ -7397,7 +7397,7 @@
         <v>R-WH_Apt_LPG*</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A90" s="32" t="s">
         <v>244</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>R-WH_Apt_ELC*</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A91" s="33" t="s">
         <v>1</v>
       </c>
@@ -7445,7 +7445,7 @@
         <v>R-WH_Apt_KER*</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A92" s="32" t="s">
         <v>1</v>
       </c>
@@ -7469,7 +7469,7 @@
         <v>R-WH_Apt_GAS*</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A93" s="33" t="s">
         <v>1</v>
       </c>
@@ -7493,7 +7493,7 @@
         <v>R-WH_Apt_PEA*</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A94" s="32" t="s">
         <v>1</v>
       </c>
@@ -7517,7 +7517,7 @@
         <v>R-WH_Apt_SMF*</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A95" s="33" t="s">
         <v>1</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>R-WH_Apt_WOO*</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A96" s="32" t="s">
         <v>1</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>R-WH_Apt_HET*</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A97" s="32" t="s">
         <v>244</v>
       </c>
@@ -7589,7 +7589,7 @@
         <v>R-WH_Apt_SOL*</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A98" s="29" t="s">
         <v>116</v>
       </c>
@@ -7601,7 +7601,7 @@
       <c r="G98" s="30"/>
       <c r="H98" s="30"/>
     </row>
-    <row r="99" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A99" s="32" t="s">
         <v>1</v>
       </c>
@@ -7625,7 +7625,7 @@
         <v>R-WH_Att_COA*</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A100" s="33" t="s">
         <v>1</v>
       </c>
@@ -7649,7 +7649,7 @@
         <v>R-WH_Att_BDL*</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A101" s="32" t="s">
         <v>1</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>R-WH_Att_ETH*</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A102" s="33" t="s">
         <v>1</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>R-WH_Att_LPG*</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A103" s="32" t="s">
         <v>244</v>
       </c>
@@ -7721,7 +7721,7 @@
         <v>R-WH_Att_ELC*X0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A104" s="33" t="s">
         <v>1</v>
       </c>
@@ -7745,7 +7745,7 @@
         <v>R-WH_Att_KER*</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A105" s="32" t="s">
         <v>1</v>
       </c>
@@ -7769,7 +7769,7 @@
         <v>R-WH_Att_GAS*</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A106" s="33" t="s">
         <v>1</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>R-WH_Att_PEA*</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A107" s="32" t="s">
         <v>1</v>
       </c>
@@ -7817,7 +7817,7 @@
         <v>R-WH_Att_SMF*</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A108" s="33" t="s">
         <v>1</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>R-WH_Att_WOO*</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A109" s="32" t="s">
         <v>1</v>
       </c>
@@ -7865,7 +7865,7 @@
         <v>R-WH_Att_HET*</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A110" s="32" t="s">
         <v>244</v>
       </c>
@@ -7889,7 +7889,7 @@
         <v>R-WH_Att_SOL*</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A111" s="29" t="s">
         <v>117</v>
       </c>
@@ -7901,7 +7901,7 @@
       <c r="G111" s="30"/>
       <c r="H111" s="30"/>
     </row>
-    <row r="112" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A112" s="32" t="s">
         <v>1</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>R-WH_Det_COA*</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A113" s="33" t="s">
         <v>1</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>R-WH_Det_BDL*</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A114" s="32" t="s">
         <v>1</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>R-WH_Det_ETH*</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A115" s="33" t="s">
         <v>1</v>
       </c>
@@ -7997,7 +7997,7 @@
         <v>R-WH_Det_LPG*</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A116" s="32" t="s">
         <v>244</v>
       </c>
@@ -8021,7 +8021,7 @@
         <v>R-WH_Det_ELC*X0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A117" s="33" t="s">
         <v>1</v>
       </c>
@@ -8045,7 +8045,7 @@
         <v>R-WH_Det_KER*</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A118" s="32" t="s">
         <v>1</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>R-WH_Det_GAS*</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A119" s="33" t="s">
         <v>1</v>
       </c>
@@ -8093,7 +8093,7 @@
         <v>R-WH_Det_PEA*</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A120" s="32" t="s">
         <v>1</v>
       </c>
@@ -8117,7 +8117,7 @@
         <v>R-WH_Det_SMF*</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A121" s="33" t="s">
         <v>1</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>R-WH_Det_WOO*</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A122" s="32" t="s">
         <v>1</v>
       </c>
@@ -8165,7 +8165,7 @@
         <v>R-WH_Det_HET*</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A123" s="32" t="s">
         <v>244</v>
       </c>
@@ -8189,7 +8189,7 @@
         <v>R-WH_Det_SOL*</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A124" s="29" t="s">
         <v>246</v>
       </c>
@@ -8201,7 +8201,7 @@
       <c r="G124" s="30"/>
       <c r="H124" s="30"/>
     </row>
-    <row r="125" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A125" s="32" t="s">
         <v>78</v>
       </c>
@@ -8225,7 +8225,7 @@
         <v>R-SH_Apt_ELC*X1</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A126" s="32" t="s">
         <v>78</v>
       </c>
@@ -8249,7 +8249,7 @@
         <v>R-SH_Att_ELC*X1</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A127" s="32" t="s">
         <v>78</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>R-SH_Det_ELC*X1</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A128" s="29" t="s">
         <v>247</v>
       </c>
@@ -8285,7 +8285,7 @@
       <c r="G128" s="30"/>
       <c r="H128" s="30"/>
     </row>
-    <row r="129" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A129" s="32" t="s">
         <v>245</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>R-SH_Apt_ELC*X1</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A130" s="32" t="s">
         <v>245</v>
       </c>
@@ -8339,7 +8339,7 @@
         <v>R-SH_Att_ELC*X1</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A131" s="38" t="s">
         <v>245</v>
       </c>
@@ -8366,7 +8366,7 @@
         <v>R-SH_Det_ELC*X1</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A132" s="29" t="s">
         <v>252</v>
       </c>
@@ -8378,7 +8378,7 @@
       <c r="G132" s="30"/>
       <c r="H132" s="30"/>
     </row>
-    <row r="133" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A133" s="32" t="s">
         <v>245</v>
       </c>
@@ -8405,7 +8405,7 @@
         <v>R-SH_Apt_ELC*X1</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A134" s="32" t="s">
         <v>245</v>
       </c>
@@ -8432,7 +8432,7 @@
         <v>R-SH_Att_ELC*X1</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A135" s="38" t="s">
         <v>245</v>
       </c>
@@ -8476,32 +8476,32 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="22"/>
-    <col min="5" max="5" width="11.140625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="22" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="13.7265625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="22"/>
+    <col min="5" max="5" width="11.1796875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="23.54296875" style="22" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" style="22" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="23.5" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="23"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="E3" s="34" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>79</v>
       </c>
@@ -8521,7 +8521,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
@@ -8531,7 +8531,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="31"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
         <v>109</v>
       </c>
@@ -8554,7 +8554,7 @@
         <v>*0.590188034188034</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>109</v>
       </c>
@@ -8577,7 +8577,7 @@
         <v>*0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
         <v>109</v>
       </c>
@@ -8600,7 +8600,7 @@
         <v>*0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
         <v>109</v>
       </c>
@@ -8623,7 +8623,7 @@
         <v>*0.806779026217228</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="32" t="s">
         <v>109</v>
       </c>
@@ -8646,7 +8646,7 @@
         <v>*3.07019607843137</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="33" t="s">
         <v>109</v>
       </c>
@@ -8669,7 +8669,7 @@
         <v>*0.810162162162162</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="32" t="s">
         <v>109</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>*0.810268817204301</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
         <v>109</v>
       </c>
@@ -8715,7 +8715,7 @@
         <v>*0.525</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="32" t="s">
         <v>109</v>
       </c>
@@ -8738,7 +8738,7 @@
         <v>*0.581777777777778</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="33" t="s">
         <v>109</v>
       </c>
@@ -8761,7 +8761,7 @@
         <v>*0.688045112781955</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="32" t="s">
         <v>109</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>*0.3983844218765</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="32" t="s">
         <v>109</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>*1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
@@ -8817,7 +8817,7 @@
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
     </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="32" t="s">
         <v>105</v>
       </c>
@@ -8840,7 +8840,7 @@
         <v>*0.557980879057327</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="33" t="s">
         <v>105</v>
       </c>
@@ -8863,7 +8863,7 @@
         <v>*1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="32" t="s">
         <v>105</v>
       </c>
@@ -8886,7 +8886,7 @@
         <v>*0.9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="33" t="s">
         <v>105</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>*0.807075774336283</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="32" t="s">
         <v>105</v>
       </c>
@@ -8932,7 +8932,7 @@
         <v>*3.11576271186441</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="33" t="s">
         <v>105</v>
       </c>
@@ -8955,7 +8955,7 @@
         <v>*0.819415584415584</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="32" t="s">
         <v>105</v>
       </c>
@@ -8978,7 +8978,7 @@
         <v>*0.817294117647059</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
         <v>105</v>
       </c>
@@ -9001,7 +9001,7 @@
         <v>*0.550929487179487</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="32" t="s">
         <v>105</v>
       </c>
@@ -9024,7 +9024,7 @@
         <v>*0.571137724550898</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="33" t="s">
         <v>105</v>
       </c>
@@ -9047,7 +9047,7 @@
         <v>*0.704006568144499</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="32" t="s">
         <v>105</v>
       </c>
@@ -9070,7 +9070,7 @@
         <v>*0.609499730599684</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="32" t="s">
         <v>105</v>
       </c>
@@ -9093,7 +9093,7 @@
         <v>*1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A31" s="30"/>
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
@@ -9103,7 +9103,7 @@
       <c r="F31" s="30"/>
       <c r="G31" s="30"/>
     </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="32" t="s">
         <v>114</v>
       </c>
@@ -9127,7 +9127,7 @@
       </c>
       <c r="H32" s="25"/>
     </row>
-    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="33" t="s">
         <v>114</v>
       </c>
@@ -9152,7 +9152,7 @@
       </c>
       <c r="H33" s="25"/>
     </row>
-    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="32" t="s">
         <v>114</v>
       </c>
@@ -9175,7 +9175,7 @@
         <v>*0.9</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="33" t="s">
         <v>114</v>
       </c>
@@ -9198,7 +9198,7 @@
         <v>*0.826617747626993</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="32" t="s">
         <v>114</v>
       </c>
@@ -9221,7 +9221,7 @@
         <v>*3.08978378378378</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="33" t="s">
         <v>114</v>
       </c>
@@ -9244,7 +9244,7 @@
         <v>*0.822803738317757</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="32" t="s">
         <v>114</v>
       </c>
@@ -9267,7 +9267,7 @@
         <v>*0.827287581699346</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="33" t="s">
         <v>114</v>
       </c>
@@ -9290,7 +9290,7 @@
         <v>*0.545789473684211</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="32" t="s">
         <v>114</v>
       </c>
@@ -9313,7 +9313,7 @@
         <v>*0.614742268041237</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="33" t="s">
         <v>114</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>*0.729286096921694</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="32" t="s">
         <v>114</v>
       </c>
@@ -9359,7 +9359,7 @@
         <v>*0.65865731206453</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="32" t="s">
         <v>114</v>
       </c>
@@ -9382,7 +9382,7 @@
         <v>*0.999520958083832</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A44" s="30"/>
       <c r="B44" s="30"/>
       <c r="C44" s="30"/>
@@ -9392,7 +9392,7 @@
       <c r="F44" s="30"/>
       <c r="G44" s="31"/>
     </row>
-    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="32" t="s">
         <v>109</v>
       </c>
@@ -9415,7 +9415,7 @@
         <v>*3.07019607843137</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="32" t="s">
         <v>105</v>
       </c>
@@ -9438,7 +9438,7 @@
         <v>*3.11576271186441</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="38" t="s">
         <v>114</v>
       </c>
@@ -9461,7 +9461,7 @@
         <v>*3.08978378378378</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A48" s="30"/>
       <c r="B48" s="30"/>
       <c r="C48" s="30"/>
@@ -9471,7 +9471,7 @@
       <c r="F48" s="30"/>
       <c r="G48" s="31"/>
     </row>
-    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="32" t="s">
         <v>109</v>
       </c>
@@ -9494,7 +9494,7 @@
         <v>*0.590188034188034</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="33" t="s">
         <v>109</v>
       </c>
@@ -9517,7 +9517,7 @@
         <v>*0.9</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="32" t="s">
         <v>109</v>
       </c>
@@ -9540,7 +9540,7 @@
         <v>*0.9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="33" t="s">
         <v>109</v>
       </c>
@@ -9563,7 +9563,7 @@
         <v>*0.806779026217228</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="32" t="s">
         <v>109</v>
       </c>
@@ -9586,7 +9586,7 @@
         <v>*1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" s="32" t="s">
         <v>109</v>
       </c>
@@ -9609,7 +9609,7 @@
         <v>*3.07019607843137</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A55" s="33" t="s">
         <v>109</v>
       </c>
@@ -9632,7 +9632,7 @@
         <v>*0.810162162162162</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="32" t="s">
         <v>109</v>
       </c>
@@ -9655,7 +9655,7 @@
         <v>*0.810268817204301</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="33" t="s">
         <v>109</v>
       </c>
@@ -9678,7 +9678,7 @@
         <v>*0.525</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="32" t="s">
         <v>109</v>
       </c>
@@ -9701,7 +9701,7 @@
         <v>*0.581777777777778</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" s="33" t="s">
         <v>109</v>
       </c>
@@ -9724,7 +9724,7 @@
         <v>*0.688045112781955</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A60" s="32" t="s">
         <v>109</v>
       </c>
@@ -9747,7 +9747,7 @@
         <v>*0.3983844218765</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A61" s="33" t="s">
         <v>109</v>
       </c>
@@ -9770,7 +9770,7 @@
         <v>*1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A62" s="30"/>
       <c r="B62" s="30"/>
       <c r="C62" s="30"/>
@@ -9780,7 +9780,7 @@
       <c r="F62" s="30"/>
       <c r="G62" s="31"/>
     </row>
-    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A63" s="32" t="s">
         <v>105</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>*0.557980879057327</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A64" s="33" t="s">
         <v>105</v>
       </c>
@@ -9826,7 +9826,7 @@
         <v>*1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A65" s="32" t="s">
         <v>105</v>
       </c>
@@ -9849,7 +9849,7 @@
         <v>*0.9</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A66" s="33" t="s">
         <v>105</v>
       </c>
@@ -9872,7 +9872,7 @@
         <v>*0.807075774336283</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A67" s="32" t="s">
         <v>105</v>
       </c>
@@ -9895,7 +9895,7 @@
         <v>*1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A68" s="32" t="s">
         <v>105</v>
       </c>
@@ -9918,7 +9918,7 @@
         <v>*3.11576271186441</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A69" s="33" t="s">
         <v>105</v>
       </c>
@@ -9941,7 +9941,7 @@
         <v>*0.819415584415584</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A70" s="32" t="s">
         <v>105</v>
       </c>
@@ -9964,7 +9964,7 @@
         <v>*0.817294117647059</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A71" s="33" t="s">
         <v>105</v>
       </c>
@@ -9987,7 +9987,7 @@
         <v>*0.550929487179487</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A72" s="32" t="s">
         <v>105</v>
       </c>
@@ -10010,7 +10010,7 @@
         <v>*0.571137724550898</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A73" s="33" t="s">
         <v>105</v>
       </c>
@@ -10033,7 +10033,7 @@
         <v>*0.704006568144499</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A74" s="32" t="s">
         <v>105</v>
       </c>
@@ -10056,7 +10056,7 @@
         <v>*0.609499730599684</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A75" s="33" t="s">
         <v>105</v>
       </c>
@@ -10079,7 +10079,7 @@
         <v>*1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A76" s="30"/>
       <c r="B76" s="30"/>
       <c r="C76" s="30"/>
@@ -10089,7 +10089,7 @@
       <c r="F76" s="30"/>
       <c r="G76" s="31"/>
     </row>
-    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A77" s="32" t="s">
         <v>114</v>
       </c>
@@ -10112,7 +10112,7 @@
         <v>*0.619863294600137</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A78" s="33" t="s">
         <v>114</v>
       </c>
@@ -10135,7 +10135,7 @@
         <v>*0.9</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A79" s="32" t="s">
         <v>114</v>
       </c>
@@ -10158,7 +10158,7 @@
         <v>*0.9</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A80" s="33" t="s">
         <v>114</v>
       </c>
@@ -10181,7 +10181,7 @@
         <v>*0.826617747626993</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A81" s="32" t="s">
         <v>114</v>
       </c>
@@ -10204,7 +10204,7 @@
         <v>*0.999520958083832</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A82" s="32" t="s">
         <v>114</v>
       </c>
@@ -10227,7 +10227,7 @@
         <v>*3.08978378378378</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A83" s="33" t="s">
         <v>114</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>*0.822803738317757</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A84" s="32" t="s">
         <v>114</v>
       </c>
@@ -10273,7 +10273,7 @@
         <v>*0.827287581699346</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A85" s="33" t="s">
         <v>114</v>
       </c>
@@ -10296,7 +10296,7 @@
         <v>*0.545789473684211</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A86" s="32" t="s">
         <v>114</v>
       </c>
@@ -10319,7 +10319,7 @@
         <v>*0.614742268041237</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A87" s="33" t="s">
         <v>114</v>
       </c>
@@ -10342,7 +10342,7 @@
         <v>*0.729286096921694</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A88" s="32" t="s">
         <v>114</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>*0.65865731206453</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A89" s="33" t="s">
         <v>114</v>
       </c>
@@ -10402,12 +10402,12 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -10489,7 +10489,7 @@
         <v>7.5051369863013695E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -10530,7 +10530,7 @@
         <v>0.45255796882634303</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -10571,7 +10571,7 @@
         <v>6.2549233288808403E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -10612,7 +10612,7 @@
         <v>1.5052975614548401</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -10653,7 +10653,7 @@
         <v>9.0422374429223698E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -10694,7 +10694,7 @@
         <v>7.5045615347050301E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -10735,7 +10735,7 @@
         <v>3.2373195740855901E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -10776,7 +10776,7 @@
         <v>0.112170033510623</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -10817,7 +10817,7 @@
         <v>0.13251764473730199</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -10858,7 +10858,7 @@
         <v>9.0627195293291204E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -10899,7 +10899,7 @@
         <v>9.0196313138344295E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -10940,7 +10940,7 @@
         <v>0.143159113753899</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -10981,7 +10981,7 @@
         <v>0.10316120676872401</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -11022,7 +11022,7 @@
         <v>8.8919330289193299E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -11063,7 +11063,7 @@
         <v>0.104359857576634</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -11104,7 +11104,7 @@
         <v>6.6402541005538801E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -11145,7 +11145,7 @@
         <v>0.66825318875216799</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -11186,7 +11186,7 @@
         <v>6.7212328767123297E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -11227,7 +11227,7 @@
         <v>5.8388567987470399E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -11268,7 +11268,7 @@
         <v>4.8794584261943399E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -11309,7 +11309,7 @@
         <v>6.9705277866978901E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -11350,7 +11350,7 @@
         <v>0.100567418678171</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -11391,7 +11391,7 @@
         <v>6.8944308925102102E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -11432,7 +11432,7 @@
         <v>5.9040638752358897E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -11473,7 +11473,7 @@
         <v>0.220198275095671</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -11514,7 +11514,7 @@
         <v>6.8778139627583307E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -11555,7 +11555,7 @@
         <v>4.2328767123287703E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -11596,7 +11596,7 @@
         <v>7.2518315131287606E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -11637,7 +11637,7 @@
         <v>4.65144570452133E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -11678,7 +11678,7 @@
         <v>0.45983560612562002</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -11719,7 +11719,7 @@
         <v>4.7947345890410997E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -11760,7 +11760,7 @@
         <v>4.6985228618266699E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -11801,7 +11801,7 @@
         <v>5.1032329364559198E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -11842,7 +11842,7 @@
         <v>5.3657823067608502E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -11883,7 +11883,7 @@
         <v>6.8787509731139299E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -11924,7 +11924,7 @@
         <v>2.36315789189348E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -11965,7 +11965,7 @@
         <v>4.4737576657325098E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -12006,7 +12006,7 @@
         <v>0.145588074596397</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -12058,12 +12058,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -12104,7 +12104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>9.4570753703752605E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -12186,7 +12186,7 @@
         <v>0.41882471081785599</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -12227,7 +12227,7 @@
         <v>1.7227618659613701E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -12268,7 +12268,7 @@
         <v>0.183575067201909</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -12309,7 +12309,7 @@
         <v>2.0352386019458902E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -12350,7 +12350,7 @@
         <v>2.5069945114006401E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -12391,7 +12391,7 @@
         <v>2.3488908827814098E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -12432,7 +12432,7 @@
         <v>7.8978154557043795E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -12473,7 +12473,7 @@
         <v>4.8787825956958103E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -12514,7 +12514,7 @@
         <v>0.15828050607333199</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -12555,7 +12555,7 @@
         <v>0.14698298838932999</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -12596,7 +12596,7 @@
         <v>3.7307426022765301E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -12637,7 +12637,7 @@
         <v>2.4658929270483999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -12678,7 +12678,7 @@
         <v>0.31784775894057798</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -12719,7 +12719,7 @@
         <v>3.7537381358533697E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -12760,7 +12760,7 @@
         <v>0.113204385544111</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -12801,7 +12801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -12842,7 +12842,7 @@
         <v>3.5032805879028399E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -12883,7 +12883,7 @@
         <v>2.2872893208017001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -12924,7 +12924,7 @@
         <v>4.4978376179101401E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -12965,7 +12965,7 @@
         <v>4.9050090196469498E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -13006,7 +13006,7 @@
         <v>7.0893554801410602E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -13047,7 +13047,7 @@
         <v>7.3631430941555998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -13088,7 +13088,7 @@
         <v>0.119017735973187</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -13129,7 +13129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -13170,7 +13170,7 @@
         <v>0.47278411842156098</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -13211,7 +13211,7 @@
         <v>4.5630448521753401E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -13252,7 +13252,7 @@
         <v>0.13766734761320301</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -13293,7 +13293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -13334,7 +13334,7 @@
         <v>3.9151690301129402E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -13375,7 +13375,7 @@
         <v>0.200825091733705</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -13416,7 +13416,7 @@
         <v>4.92788432018662E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -13457,7 +13457,7 @@
         <v>7.0854130591549894E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -13498,7 +13498,7 @@
         <v>0.100420210433235</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -13539,7 +13539,7 @@
         <v>0.13720876081054401</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -13591,12 +13591,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -13637,7 +13637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -13678,7 +13678,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -13719,7 +13719,7 @@
         <v>0.59018803418803401</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -13760,7 +13760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -13801,7 +13801,7 @@
         <v>3.07019607843137</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -13842,7 +13842,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -13883,7 +13883,7 @@
         <v>0.810268817204301</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -13924,7 +13924,7 @@
         <v>0.39838442187649997</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -13965,7 +13965,7 @@
         <v>0.81016216216216197</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -14006,7 +14006,7 @@
         <v>0.80677902621722797</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -14047,7 +14047,7 @@
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -14088,7 +14088,7 @@
         <v>0.58177777777777795</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -14129,7 +14129,7 @@
         <v>0.68804511278195502</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -14170,7 +14170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -14211,7 +14211,7 @@
         <v>0.55798087905732696</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -14252,7 +14252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -14293,7 +14293,7 @@
         <v>3.1157627118644098</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -14334,7 +14334,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -14375,7 +14375,7 @@
         <v>0.81729411764705895</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -14416,7 +14416,7 @@
         <v>0.60949973059968399</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -14457,7 +14457,7 @@
         <v>0.81941558441558404</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -14498,7 +14498,7 @@
         <v>0.80707577433628297</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -14539,7 +14539,7 @@
         <v>0.55092948717948698</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -14580,7 +14580,7 @@
         <v>0.57113772455089795</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -14621,7 +14621,7 @@
         <v>0.70400656814449902</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -14662,7 +14662,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -14703,7 +14703,7 @@
         <v>0.619863294600137</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -14744,7 +14744,7 @@
         <v>0.99952095808383201</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -14785,7 +14785,7 @@
         <v>3.0897837837837798</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -14826,7 +14826,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -14867,7 +14867,7 @@
         <v>0.82728758169934602</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -14908,7 +14908,7 @@
         <v>0.65865731206453004</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -14949,7 +14949,7 @@
         <v>0.82280373831775699</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -14990,7 +14990,7 @@
         <v>0.82661774762699303</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -15031,7 +15031,7 @@
         <v>0.54578947368421105</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -15072,7 +15072,7 @@
         <v>0.61474226804123699</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -15113,7 +15113,7 @@
         <v>0.72928609692169399</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -15154,7 +15154,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -15195,7 +15195,7 @@
         <v>0.59018803418803401</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -15236,7 +15236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -15277,7 +15277,7 @@
         <v>3.07019607843137</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -15318,7 +15318,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -15359,7 +15359,7 @@
         <v>0.810268817204301</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>77</v>
       </c>
@@ -15400,7 +15400,7 @@
         <v>0.39838442187649997</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -15441,7 +15441,7 @@
         <v>0.81016216216216197</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>77</v>
       </c>
@@ -15482,7 +15482,7 @@
         <v>0.80677902621722797</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>77</v>
       </c>
@@ -15523,7 +15523,7 @@
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -15564,7 +15564,7 @@
         <v>0.58177777777777795</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>77</v>
       </c>
@@ -15605,7 +15605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -15646,7 +15646,7 @@
         <v>0.68804511278195502</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>77</v>
       </c>
@@ -15687,7 +15687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>77</v>
       </c>
@@ -15728,7 +15728,7 @@
         <v>0.55798087905732696</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>77</v>
       </c>
@@ -15769,7 +15769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>77</v>
       </c>
@@ -15810,7 +15810,7 @@
         <v>3.1157627118644098</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>77</v>
       </c>
@@ -15851,7 +15851,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -15892,7 +15892,7 @@
         <v>0.81729411764705895</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>77</v>
       </c>
@@ -15933,7 +15933,7 @@
         <v>0.60949973059968399</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -15974,7 +15974,7 @@
         <v>0.81941558441558404</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>77</v>
       </c>
@@ -16015,7 +16015,7 @@
         <v>0.80707577433628297</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>77</v>
       </c>
@@ -16056,7 +16056,7 @@
         <v>0.55092948717948698</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>77</v>
       </c>
@@ -16097,7 +16097,7 @@
         <v>0.57113772455089795</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -16138,7 +16138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -16179,7 +16179,7 @@
         <v>0.70400656814449902</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -16220,7 +16220,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -16261,7 +16261,7 @@
         <v>0.619863294600137</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -16302,7 +16302,7 @@
         <v>0.99952095808383201</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>77</v>
       </c>
@@ -16343,7 +16343,7 @@
         <v>3.0897837837837798</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -16384,7 +16384,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -16425,7 +16425,7 @@
         <v>0.82728758169934602</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -16466,7 +16466,7 @@
         <v>0.65865731206453004</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -16507,7 +16507,7 @@
         <v>0.82280373831775699</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -16548,7 +16548,7 @@
         <v>0.82661774762699303</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -16589,7 +16589,7 @@
         <v>0.54578947368421105</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -16630,7 +16630,7 @@
         <v>0.61474226804123699</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>77</v>
       </c>
@@ -16671,7 +16671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Update new energy security scenarios
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIM-2.0\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4CC272-783F-4708-92ED-B82517C62AED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A96F820-4A56-4017-B391-79467CF1423B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1450" yWindow="830" windowWidth="14400" windowHeight="7360" tabRatio="819" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" tabRatio="819" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="64" r:id="rId1"/>

</xml_diff>

<commit_message>
Update very high natural gas price scenario
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIM-2.0\TIM\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIM-2.0\TIMES-Ireland-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A96F820-4A56-4017-B391-79467CF1423B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B3D572-8EA5-47E6-B7E6-DA5D5BBC63AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" tabRatio="819" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23856" yWindow="4116" windowWidth="14400" windowHeight="7356" tabRatio="819" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="64" r:id="rId1"/>

</xml_diff>